<commit_message>
corte de caja report
</commit_message>
<xml_diff>
--- a/public/reportTemplates/template-corte-caja.xlsx
+++ b/public/reportTemplates/template-corte-caja.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorgeivangomez/Documents/Projects/DELFINITI/delfiniti-app/public/reportTemplates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F923E4-2AEC-7840-A52A-72E369354AF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90ACC9A-3C59-3D4C-96CD-A78BD378E07C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="900" yWindow="500" windowWidth="28800" windowHeight="16580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,15 +32,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Delfiniti de México S.A. de C.V.</t>
   </si>
   <si>
     <t>Corte de caja</t>
-  </si>
-  <si>
-    <t>Del viernes 24/junio/2022 al viernes 24/junio/2022</t>
   </si>
 </sst>
 </file>
@@ -117,13 +114,13 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -433,7 +430,7 @@
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -448,15 +445,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -467,15 +464,15 @@
       <c r="O1" s="2"/>
     </row>
     <row r="2" spans="1:15" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -486,15 +483,13 @@
       <c r="O2" s="3"/>
     </row>
     <row r="3" spans="1:15" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>

</xml_diff>